<commit_message>
Almost final long file
</commit_message>
<xml_diff>
--- a/balanced_dataset_results_UPDATED.xlsx
+++ b/balanced_dataset_results_UPDATED.xlsx
@@ -1,29 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#coding ground\Github\Repos\fraud_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4CD6D8-BB0A-48DD-B126-BF20B08131C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11D767D-D93D-48C8-9E06-8FF71280883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4350" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
     <sheet name="Class_weight" sheetId="2" r:id="rId2"/>
     <sheet name="SMOTECNC_dataset" sheetId="3" r:id="rId3"/>
     <sheet name="main" sheetId="4" r:id="rId4"/>
+    <sheet name="import" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="56">
   <si>
     <t>fbeta</t>
   </si>
@@ -219,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +243,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -282,9 +314,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -292,7 +321,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -601,9 +652,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -664,7 +715,7 @@
         <v>0.383087158203125</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -696,7 +747,7 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -728,7 +779,7 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -760,7 +811,7 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -792,7 +843,7 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -824,7 +875,7 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -856,7 +907,7 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -888,7 +939,7 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -920,7 +971,7 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -965,9 +1016,9 @@
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -996,8 +1047,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1031,8 +1082,8 @@
         <v>0.383087158203125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1064,8 +1115,8 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1097,8 +1148,8 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1130,8 +1181,8 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1163,8 +1214,8 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1196,8 +1247,8 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1229,8 +1280,8 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1262,8 +1313,8 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1295,8 +1346,8 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1328,8 +1379,8 @@
         <v>3.2007455825805657E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1363,8 +1414,8 @@
         <v>0.40109086036682129</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1396,8 +1447,8 @@
         <v>0.34207820892333979</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1429,8 +1480,8 @@
         <v>1.10018253326416E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1462,8 +1513,8 @@
         <v>0.35908150672912598</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1495,8 +1546,8 @@
         <v>0.28206443786621088</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1528,8 +1579,8 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1561,8 +1612,8 @@
         <v>0.39809083938598627</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1594,8 +1645,8 @@
         <v>0.33907699584960938</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1627,8 +1678,8 @@
         <v>1.100277900695801E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1660,8 +1711,8 @@
         <v>0.36808395385742188</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
@@ -1693,8 +1744,8 @@
         <v>0.28406572341918951</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1726,8 +1777,8 @@
         <v>1.1002302169799799E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1761,8 +1812,8 @@
         <v>0.46810579299926758</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1794,8 +1845,8 @@
         <v>0.47099637985229492</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1827,8 +1878,8 @@
         <v>1.3003110885620121E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1860,8 +1911,8 @@
         <v>15.430972099304199</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1893,8 +1944,8 @@
         <v>5.5012226104736328E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
@@ -1926,8 +1977,8 @@
         <v>0.5391232967376709</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1959,8 +2010,8 @@
         <v>8.6019277572631836E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1992,8 +2043,8 @@
         <v>4.7031164169311523E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
@@ -2025,8 +2076,8 @@
         <v>3.4007549285888672E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
       <c r="B33" s="1" t="s">
         <v>18</v>
       </c>
@@ -2058,8 +2109,8 @@
         <v>3.3007383346557617E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2093,8 +2144,8 @@
         <v>0.3140714168548584</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
       <c r="B35" s="1" t="s">
         <v>10</v>
       </c>
@@ -2126,8 +2177,8 @@
         <v>0.32007265090942377</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
       <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
@@ -2159,8 +2210,8 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37" s="1" t="s">
         <v>12</v>
       </c>
@@ -2192,8 +2243,8 @@
         <v>14.614700794219971</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
@@ -2225,8 +2276,8 @@
         <v>5.5012702941894531E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2258,8 +2309,8 @@
         <v>0.50911545753479004</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
       <c r="B40" s="1" t="s">
         <v>15</v>
       </c>
@@ -2291,8 +2342,8 @@
         <v>7.3016881942749023E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
@@ -2324,8 +2375,8 @@
         <v>3.8009405136108398E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
       <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
@@ -2357,8 +2408,8 @@
         <v>3.2007217407226563E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
       <c r="B43" s="1" t="s">
         <v>18</v>
       </c>
@@ -2409,14 +2460,14 @@
       <selection activeCell="A16" sqref="A16:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2436,7 +2487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2459,7 +2510,7 @@
         <v>0.53429231954790646</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2482,7 +2533,7 @@
         <v>0.91261952146719916</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2505,7 +2556,7 @@
         <v>5.1847051198963059E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -2528,7 +2579,7 @@
         <v>0.85106382978723405</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -2551,7 +2602,7 @@
         <v>0.69808028329850547</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2574,7 +2625,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2597,7 +2648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2620,7 +2671,7 @@
         <v>2829.5603652000432</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -2643,7 +2694,7 @@
         <v>0.1520347595214844</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2666,7 +2717,7 @@
         <v>0.14903450012207031</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2698,7 +2749,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -2733,7 +2784,7 @@
         <v>1.10015869140625E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2768,7 +2819,7 @@
         <v>74.969163417816162</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -2803,7 +2854,7 @@
         <v>6.3014507293701172E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2838,7 +2889,7 @@
         <v>1.032234668731689</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -2873,7 +2924,7 @@
         <v>5.9012651443481452E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -2915,27 +2966,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD01605-4AAB-4FF0-9739-8536CB6D4A68}">
-  <dimension ref="B2:M63"/>
+  <dimension ref="A2:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2964,11 +3016,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>AVERAGE(D3:D12)</f>
+        <v>0.76506404331409994</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D3">
@@ -2986,10 +3042,10 @@
       <c r="H3">
         <v>0.798396406951702</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="12">
         <v>27</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <v>20</v>
       </c>
       <c r="K3">
@@ -2998,12 +3054,15 @@
       <c r="L3">
         <v>14.614700794219971</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D4">
@@ -3021,10 +3080,10 @@
       <c r="H4">
         <v>0.69266409513752059</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="12">
         <v>20</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="12">
         <v>21</v>
       </c>
       <c r="K4">
@@ -3033,12 +3092,15 @@
       <c r="L4">
         <v>1.1002302169799799E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="M4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D5">
@@ -3059,7 +3121,7 @@
       <c r="I5">
         <v>162</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="10">
         <v>17</v>
       </c>
       <c r="K5">
@@ -3068,12 +3130,15 @@
       <c r="L5">
         <v>15.430972099304199</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="M5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D6">
@@ -3091,10 +3156,10 @@
       <c r="H6">
         <v>0.79517925129512146</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="10">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="10">
         <v>22</v>
       </c>
       <c r="K6">
@@ -3103,12 +3168,15 @@
       <c r="L6">
         <v>0.46810579299926758</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="M6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D7">
@@ -3126,10 +3194,10 @@
       <c r="H7">
         <v>0.7956550709889284</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="10">
         <v>5</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="10">
         <v>22</v>
       </c>
       <c r="K7">
@@ -3138,8 +3206,11 @@
       <c r="L7">
         <v>0.47099637985229492</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3173,8 +3244,11 @@
       <c r="L8">
         <v>1.100254058837891E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
@@ -3208,13 +3282,16 @@
       <c r="L9">
         <v>3.8009405136108398E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>0.75051546391752577</v>
@@ -3229,7 +3306,7 @@
         <v>0.74468085106382975</v>
       </c>
       <c r="H10">
-        <v>0.78138405242704723</v>
+        <v>0.79148001643310684</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -3238,18 +3315,21 @@
         <v>24</v>
       </c>
       <c r="K10">
-        <v>111.7752957344055</v>
+        <v>14.24628615379333</v>
       </c>
       <c r="L10">
-        <v>0.39809083938598627</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+        <v>3.2007217407226563E-2</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>0.75051546391752577</v>
@@ -3264,7 +3344,7 @@
         <v>0.74468085106382975</v>
       </c>
       <c r="H11">
-        <v>0.79148001643310684</v>
+        <v>0.78138405242704723</v>
       </c>
       <c r="I11">
         <v>5</v>
@@ -3273,13 +3353,13 @@
         <v>24</v>
       </c>
       <c r="K11">
-        <v>14.24628615379333</v>
+        <v>111.7752957344055</v>
       </c>
       <c r="L11">
-        <v>3.2007217407226563E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.39809083938598627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3301,10 +3381,10 @@
       <c r="H12">
         <v>0.7965227694974365</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="10">
         <v>10</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="10">
         <v>24</v>
       </c>
       <c r="K12">
@@ -3314,7 +3394,11 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>AVERAGE(D13:D22)</f>
+        <v>0.73055183944449764</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3336,10 +3420,10 @@
       <c r="H13">
         <v>0.75430066832260534</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <v>15</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="10">
         <v>24</v>
       </c>
       <c r="K13">
@@ -3349,7 +3433,7 @@
         <v>3.4007549285888672E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
@@ -3371,10 +3455,10 @@
       <c r="H14">
         <v>0.7416169653365382</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="10">
         <v>24</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="10">
         <v>24</v>
       </c>
       <c r="K14">
@@ -3384,7 +3468,7 @@
         <v>4.7031164169311523E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -3406,10 +3490,10 @@
       <c r="H15">
         <v>0.6529289272415072</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="10">
         <v>66</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="10">
         <v>23</v>
       </c>
       <c r="K15">
@@ -3419,12 +3503,12 @@
         <v>1.3003110885620121E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <v>0.74009900990099009</v>
@@ -3439,7 +3523,7 @@
         <v>0.73404255319148937</v>
       </c>
       <c r="H16">
-        <v>0.76922045064647449</v>
+        <v>0.78850603492058602</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -3448,18 +3532,18 @@
         <v>25</v>
       </c>
       <c r="K16">
-        <v>111.02922034263609</v>
+        <v>80.789705514907837</v>
       </c>
       <c r="L16">
-        <v>0.40109086036682129</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.3140714168548584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>0.74009900990099009</v>
@@ -3474,7 +3558,7 @@
         <v>0.73404255319148937</v>
       </c>
       <c r="H17">
-        <v>0.78850603492058602</v>
+        <v>0.76922045064647449</v>
       </c>
       <c r="I17">
         <v>5</v>
@@ -3483,13 +3567,13 @@
         <v>25</v>
       </c>
       <c r="K17">
-        <v>80.789705514907837</v>
+        <v>111.02922034263609</v>
       </c>
       <c r="L17">
-        <v>0.3140714168548584</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.40109086036682129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -3524,7 +3608,7 @@
         <v>3.5007953643798828E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3559,12 +3643,12 @@
         <v>0.36808395385742188</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D20">
         <v>0.71924029727497929</v>
@@ -3579,7 +3663,7 @@
         <v>0.71276595744680848</v>
       </c>
       <c r="H20">
-        <v>0.78470588766634308</v>
+        <v>0.78614400612430047</v>
       </c>
       <c r="I20">
         <v>5</v>
@@ -3588,18 +3672,18 @@
         <v>27</v>
       </c>
       <c r="K20">
-        <v>101.8953905105591</v>
+        <v>88.842020034790039</v>
       </c>
       <c r="L20">
-        <v>0.383087158203125</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.35908150672912598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>0.71924029727497929</v>
@@ -3614,7 +3698,7 @@
         <v>0.71276595744680848</v>
       </c>
       <c r="H21">
-        <v>0.78614400612430047</v>
+        <v>0.78470588766634308</v>
       </c>
       <c r="I21">
         <v>5</v>
@@ -3623,13 +3707,13 @@
         <v>27</v>
       </c>
       <c r="K21">
-        <v>88.842020034790039</v>
+        <v>101.8953905105591</v>
       </c>
       <c r="L21">
-        <v>0.35908150672912598</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+        <v>0.383087158203125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3664,7 +3748,11 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>AVERAGE(D23:D34)</f>
+        <v>0.64199376937573627</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
@@ -3699,7 +3787,7 @@
         <v>0.32007265090942377</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
@@ -3734,7 +3822,7 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -3769,7 +3857,7 @@
         <v>3.2007455825805657E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
@@ -3794,7 +3882,7 @@
       <c r="I26">
         <v>627</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="8">
         <v>14</v>
       </c>
       <c r="K26">
@@ -3804,7 +3892,7 @@
         <v>0.50911545753479004</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
@@ -3829,7 +3917,7 @@
       <c r="I27">
         <v>470</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="10">
         <v>19</v>
       </c>
       <c r="K27">
@@ -3839,7 +3927,7 @@
         <v>0.5391232967376709</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
@@ -3874,7 +3962,7 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
@@ -3909,7 +3997,7 @@
         <v>3.3007383346557617E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -3944,7 +4032,7 @@
         <v>0.28406572341918951</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3979,7 +4067,7 @@
         <v>0.28206443786621088</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
@@ -4014,7 +4102,7 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
@@ -4049,7 +4137,7 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
@@ -4084,7 +4172,11 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>AVERAGE(D35:D44)</f>
+        <v>0.35857142738267272</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
@@ -4109,7 +4201,7 @@
       <c r="I35">
         <v>2121</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="8">
         <v>14</v>
       </c>
       <c r="K35">
@@ -4119,7 +4211,7 @@
         <v>0.33907699584960938</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>20</v>
       </c>
@@ -4144,7 +4236,7 @@
       <c r="I36">
         <v>2132</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="8">
         <v>14</v>
       </c>
       <c r="K36">
@@ -4154,7 +4246,7 @@
         <v>0.34207820892333979</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
@@ -4189,7 +4281,7 @@
         <v>8.6019277572631836E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
@@ -4224,7 +4316,7 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
@@ -4259,7 +4351,7 @@
         <v>7.3016881942749023E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>19</v>
       </c>
@@ -4294,7 +4386,7 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>20</v>
       </c>
@@ -4329,7 +4421,7 @@
         <v>1.10018253326416E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>34</v>
       </c>
@@ -4364,7 +4456,7 @@
         <v>5.5012702941894531E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>20</v>
       </c>
@@ -4399,7 +4491,7 @@
         <v>1.100277900695801E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>33</v>
       </c>
@@ -4434,7 +4526,7 @@
         <v>5.5012226104736328E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>0</v>
       </c>
@@ -4466,336 +4558,350 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C48" s="5" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
+      <c r="C48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48">
+        <v>0.53429231954790646</v>
+      </c>
+      <c r="E48">
+        <v>0.91261952146719916</v>
+      </c>
+      <c r="F48">
+        <v>5.1847051198963059E-2</v>
+      </c>
+      <c r="G48">
+        <v>0.85106382978723405</v>
+      </c>
+      <c r="H48">
+        <v>0.69808028329850547</v>
+      </c>
+      <c r="I48">
+        <v>1463</v>
+      </c>
+      <c r="J48">
+        <v>14</v>
+      </c>
+      <c r="K48">
+        <v>2829.5603652000432</v>
+      </c>
+      <c r="L48">
+        <v>0.1520347595214844</v>
+      </c>
+      <c r="M48">
+        <v>0.14903450012207031</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="10"/>
+      <c r="C49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0.75689981096408332</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0.90765040672696617</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.26101694915254242</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0.81914893617021278</v>
+      </c>
+      <c r="H49" s="5">
+        <v>0.80113338016704927</v>
+      </c>
+      <c r="I49" s="5">
+        <v>218</v>
+      </c>
+      <c r="J49" s="5">
+        <v>17</v>
+      </c>
+      <c r="K49" s="5">
+        <v>621.48497343063354</v>
+      </c>
+      <c r="L49" s="5">
+        <v>2785.7766802310939</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="10"/>
+      <c r="C50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <v>0.63778273335457158</v>
+      </c>
+      <c r="E50">
+        <v>0.90329037777778609</v>
+      </c>
+      <c r="F50">
+        <v>9.7591888466413187E-2</v>
+      </c>
+      <c r="G50">
+        <v>0.81914893617021278</v>
+      </c>
+      <c r="H50">
+        <v>0.70210898520029352</v>
+      </c>
+      <c r="I50">
+        <v>712</v>
+      </c>
+      <c r="J50">
+        <v>17</v>
+      </c>
+      <c r="K50">
+        <v>17.717572500705721</v>
+      </c>
+      <c r="L50">
+        <v>0.85363626480102539</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D51" s="5">
         <v>0.79741727199354318</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E51" s="5">
         <v>0.90379636873323299</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F51" s="5">
         <v>0.59375</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G51" s="5">
         <v>0.80851063829787229</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H51" s="5">
         <v>0.77776653446199817</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I51" s="5">
         <v>52</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J51" s="5">
         <v>18</v>
       </c>
-      <c r="K48" s="6">
+      <c r="K51" s="5">
         <v>204.73599044481909</v>
       </c>
-      <c r="L48" s="6">
+      <c r="L51" s="5">
         <v>6.2342522144317627</v>
       </c>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C49" s="3" t="s">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="8"/>
+      <c r="C52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.76411446249033255</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.90284316402369558</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0.32203389830508472</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0.63109300844688321</v>
+      </c>
+      <c r="I52" s="5">
+        <v>160</v>
+      </c>
+      <c r="J52" s="5">
+        <v>18</v>
+      </c>
+      <c r="K52">
+        <v>6471.1831476688394</v>
+      </c>
+      <c r="L52">
+        <v>74.701642036437988</v>
+      </c>
+      <c r="M52">
+        <v>74.969163417816162</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0.77442414614773636</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0.89811535504621998</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0.44642857142857151</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0.7978723404255319</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0.6929470987941333</v>
+      </c>
+      <c r="I53" s="5">
+        <v>93</v>
+      </c>
+      <c r="J53" s="5">
+        <v>19</v>
+      </c>
+      <c r="K53">
+        <v>797.83375072479248</v>
+      </c>
+      <c r="L53">
+        <v>1.300382614135742E-2</v>
+      </c>
+      <c r="M53">
+        <v>1.10015869140625E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="10"/>
+      <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D49">
+      <c r="D54">
         <v>0.79046836483155314</v>
       </c>
-      <c r="E49">
+      <c r="E54">
         <v>0.89352876158126815</v>
       </c>
-      <c r="F49">
+      <c r="F54">
         <v>0.88095238095238093</v>
-      </c>
-      <c r="G49">
-        <v>0.78723404255319152</v>
-      </c>
-      <c r="H49">
-        <v>0.80511414406811932</v>
-      </c>
-      <c r="I49">
-        <v>10</v>
-      </c>
-      <c r="J49">
-        <v>20</v>
-      </c>
-      <c r="K49">
-        <v>628.83125205039983</v>
-      </c>
-      <c r="L49">
-        <v>1.173768281936646</v>
-      </c>
-    </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C50" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50">
-        <v>0.77978635990139689</v>
-      </c>
-      <c r="E50">
-        <v>0.88820078667556523</v>
-      </c>
-      <c r="F50">
-        <v>0.86904761904761907</v>
-      </c>
-      <c r="G50">
-        <v>0.77659574468085102</v>
-      </c>
-      <c r="H50">
-        <v>0.80735210915347733</v>
-      </c>
-      <c r="I50">
-        <v>11</v>
-      </c>
-      <c r="J50">
-        <v>21</v>
-      </c>
-      <c r="K50">
-        <v>1341.127286195755</v>
-      </c>
-      <c r="L50">
-        <v>10.52744150161743</v>
-      </c>
-    </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C51" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51">
-        <v>0.7794661190965092</v>
-      </c>
-      <c r="E51">
-        <v>0.88819196070603246</v>
-      </c>
-      <c r="F51">
-        <v>0.85882352941176465</v>
-      </c>
-      <c r="G51">
-        <v>0.77659574468085102</v>
-      </c>
-      <c r="H51">
-        <v>0.79723721826175509</v>
-      </c>
-      <c r="I51">
-        <v>12</v>
-      </c>
-      <c r="J51">
-        <v>21</v>
-      </c>
-      <c r="K51">
-        <v>589.43659858703609</v>
-      </c>
-      <c r="L51">
-        <v>1.2859871387481689</v>
-      </c>
-    </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C52" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="6">
-        <v>0.77442414614773636</v>
-      </c>
-      <c r="E52" s="6">
-        <v>0.89811535504621998</v>
-      </c>
-      <c r="F52" s="6">
-        <v>0.44642857142857151</v>
-      </c>
-      <c r="G52" s="6">
-        <v>0.7978723404255319</v>
-      </c>
-      <c r="H52" s="6">
-        <v>0.6929470987941333</v>
-      </c>
-      <c r="I52" s="6">
-        <v>93</v>
-      </c>
-      <c r="J52" s="6">
-        <v>19</v>
-      </c>
-      <c r="K52">
-        <v>797.83375072479248</v>
-      </c>
-      <c r="L52">
-        <v>1.300382614135742E-2</v>
-      </c>
-      <c r="M52">
-        <v>1.10015869140625E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="6">
-        <v>0.76411446249033255</v>
-      </c>
-      <c r="E53" s="6">
-        <v>0.90284316402369558</v>
-      </c>
-      <c r="F53" s="6">
-        <v>0.32203389830508472</v>
-      </c>
-      <c r="G53" s="6">
-        <v>0.80851063829787229</v>
-      </c>
-      <c r="H53" s="6">
-        <v>0.63109300844688321</v>
-      </c>
-      <c r="I53" s="6">
-        <v>160</v>
-      </c>
-      <c r="J53" s="6">
-        <v>18</v>
-      </c>
-      <c r="K53">
-        <v>6471.1831476688394</v>
-      </c>
-      <c r="L53">
-        <v>74.701642036437988</v>
-      </c>
-      <c r="M53">
-        <v>74.969163417816162</v>
-      </c>
-    </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C54" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54">
-        <v>0.76379515680825727</v>
-      </c>
-      <c r="E54">
-        <v>0.89277855417098428</v>
-      </c>
-      <c r="F54">
-        <v>0.43786982248520712</v>
       </c>
       <c r="G54">
         <v>0.78723404255319152</v>
       </c>
       <c r="H54">
-        <v>0.74267613697109314</v>
+        <v>0.80511414406811932</v>
       </c>
       <c r="I54">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="J54">
         <v>20</v>
       </c>
       <c r="K54">
+        <v>628.83125205039983</v>
+      </c>
+      <c r="L54">
+        <v>1.173768281936646</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55">
+        <v>0.76379515680825727</v>
+      </c>
+      <c r="E55">
+        <v>0.89277855417098428</v>
+      </c>
+      <c r="F55">
+        <v>0.43786982248520712</v>
+      </c>
+      <c r="G55">
+        <v>0.78723404255319152</v>
+      </c>
+      <c r="H55">
+        <v>0.74267613697109314</v>
+      </c>
+      <c r="I55">
+        <v>95</v>
+      </c>
+      <c r="J55">
+        <v>20</v>
+      </c>
+      <c r="K55">
         <v>4459.9327099323273</v>
       </c>
-      <c r="L54">
+      <c r="L55">
         <v>7.8017473220825195E-2</v>
       </c>
-      <c r="M54">
+      <c r="M55">
         <v>6.3014507293701172E-2</v>
       </c>
     </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C55" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="6">
-        <v>0.75689981096408332</v>
-      </c>
-      <c r="E55" s="6">
-        <v>0.90765040672696617</v>
-      </c>
-      <c r="F55" s="6">
-        <v>0.26101694915254242</v>
-      </c>
-      <c r="G55" s="6">
-        <v>0.81914893617021278</v>
-      </c>
-      <c r="H55" s="6">
-        <v>0.80113338016704927</v>
-      </c>
-      <c r="I55" s="6">
-        <v>218</v>
-      </c>
-      <c r="J55" s="6">
-        <v>17</v>
-      </c>
-      <c r="K55" s="6">
-        <v>621.48497343063354</v>
-      </c>
-      <c r="L55" s="6">
-        <v>2785.7766802310939</v>
-      </c>
-    </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" s="10"/>
       <c r="C56" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D56">
-        <v>0.75051546391752577</v>
+        <v>0.77978635990139689</v>
       </c>
       <c r="E56">
-        <v>0.87229629568425104</v>
+        <v>0.88820078667556523</v>
       </c>
       <c r="F56">
-        <v>0.93333333333333335</v>
+        <v>0.86904761904761907</v>
       </c>
       <c r="G56">
-        <v>0.74468085106382975</v>
+        <v>0.77659574468085102</v>
       </c>
       <c r="H56">
-        <v>0.78794303482881833</v>
+        <v>0.80735210915347733</v>
       </c>
       <c r="I56">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J56">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K56">
-        <v>238.5943453192711</v>
+        <v>1341.127286195755</v>
       </c>
       <c r="L56">
-        <v>1.090114831924438</v>
-      </c>
-    </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.3">
+        <v>10.52744150161743</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="10"/>
       <c r="C57" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D57">
-        <v>0.74743326488706363</v>
+        <v>0.7794661190965092</v>
       </c>
       <c r="E57">
-        <v>0.8722080359889236</v>
+        <v>0.88819196070603246</v>
       </c>
       <c r="F57">
-        <v>0.82352941176470584</v>
+        <v>0.85882352941176465</v>
       </c>
       <c r="G57">
-        <v>0.74468085106382975</v>
+        <v>0.77659574468085102</v>
       </c>
       <c r="H57">
-        <v>0.68698419987573189</v>
+        <v>0.79723721826175509</v>
       </c>
       <c r="I57">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J57">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K57">
-        <v>39.437344989776612</v>
+        <v>589.43659858703609</v>
       </c>
       <c r="L57">
-        <v>0.33799505233764648</v>
-      </c>
-    </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.3">
+        <v>1.2859871387481689</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
       <c r="C58" s="1" t="s">
         <v>38</v>
       </c>
@@ -4830,117 +4936,622 @@
         <v>1.032234668731689</v>
       </c>
     </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C59" s="1" t="s">
-        <v>39</v>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="10"/>
+      <c r="C59" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D59">
-        <v>0.71232876712328763</v>
+        <v>0.75051546391752577</v>
       </c>
       <c r="E59">
-        <v>0.87114891964499319</v>
+        <v>0.87229629568425104</v>
       </c>
       <c r="F59">
-        <v>0.34146341463414642</v>
+        <v>0.93333333333333335</v>
       </c>
       <c r="G59">
         <v>0.74468085106382975</v>
       </c>
       <c r="H59">
-        <v>0.56444419910745947</v>
+        <v>0.78794303482881833</v>
       </c>
       <c r="I59">
-        <v>135</v>
+        <v>5</v>
       </c>
       <c r="J59">
         <v>24</v>
       </c>
       <c r="K59">
+        <v>238.5943453192711</v>
+      </c>
+      <c r="L59">
+        <v>1.090114831924438</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60" s="10"/>
+      <c r="C60" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60">
+        <v>0.74743326488706363</v>
+      </c>
+      <c r="E60">
+        <v>0.8722080359889236</v>
+      </c>
+      <c r="F60">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="G60">
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="H60">
+        <v>0.68698419987573189</v>
+      </c>
+      <c r="I60">
+        <v>15</v>
+      </c>
+      <c r="J60">
+        <v>24</v>
+      </c>
+      <c r="K60">
+        <v>39.437344989776612</v>
+      </c>
+      <c r="L60">
+        <v>0.33799505233764648</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61">
+        <v>0.71232876712328763</v>
+      </c>
+      <c r="E61">
+        <v>0.87114891964499319</v>
+      </c>
+      <c r="F61">
+        <v>0.34146341463414642</v>
+      </c>
+      <c r="G61">
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="H61">
+        <v>0.56444419910745947</v>
+      </c>
+      <c r="I61">
+        <v>135</v>
+      </c>
+      <c r="J61">
+        <v>24</v>
+      </c>
+      <c r="K61">
         <v>36006.675769805908</v>
       </c>
-      <c r="L59">
+      <c r="L61">
         <v>6.1014413833618157E-2</v>
       </c>
-      <c r="M59">
+      <c r="M61">
         <v>5.9012651443481452E-2</v>
       </c>
     </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C60" s="3" t="s">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="7"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:L44">
+    <sortCondition descending="1" ref="D3:D44"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402F7E11-1355-4E9D-BD83-254983E0A558}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="16">
+        <v>0.79741727199354318</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.90379636873323299</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.59375</v>
+      </c>
+      <c r="E2" s="16">
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.77776653446199817</v>
+      </c>
+      <c r="G2" s="16">
+        <v>52</v>
+      </c>
+      <c r="H2" s="16">
+        <v>18</v>
+      </c>
+      <c r="I2" s="16">
+        <v>204.73599044481909</v>
+      </c>
+      <c r="J2" s="16">
+        <v>6.2342522144317627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.79046836483155314</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.89352876158126815</v>
+      </c>
+      <c r="D3" s="16">
+        <v>0.88095238095238093</v>
+      </c>
+      <c r="E3" s="16">
+        <v>0.78723404255319152</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0.80511414406811932</v>
+      </c>
+      <c r="G3" s="16">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16">
+        <v>20</v>
+      </c>
+      <c r="I3" s="16">
+        <v>628.83125205039983</v>
+      </c>
+      <c r="J3" s="16">
+        <v>1.173768281936646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.77978635990139689</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.88820078667556523</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.86904761904761907</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.77659574468085102</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.80735210915347733</v>
+      </c>
+      <c r="G4" s="16">
+        <v>11</v>
+      </c>
+      <c r="H4" s="16">
+        <v>21</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1341.127286195755</v>
+      </c>
+      <c r="J4" s="16">
+        <v>10.52744150161743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0.7794661190965092</v>
+      </c>
+      <c r="C5">
+        <v>0.88819196070603246</v>
+      </c>
+      <c r="D5">
+        <v>0.85882352941176465</v>
+      </c>
+      <c r="E5">
+        <v>0.77659574468085102</v>
+      </c>
+      <c r="F5">
+        <v>0.79723721826175509</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <v>589.43659858703609</v>
+      </c>
+      <c r="J5">
+        <v>1.2859871387481689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.77442414614773636</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.89811535504621998</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.44642857142857151</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.7978723404255319</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.6929470987941333</v>
+      </c>
+      <c r="G6" s="16">
+        <v>93</v>
+      </c>
+      <c r="H6" s="16">
+        <v>19</v>
+      </c>
+      <c r="I6" s="16">
+        <v>797.83375072479248</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1.300382614135742E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.76411446249033255</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.90284316402369558</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.32203389830508472</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.80851063829787229</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.63109300844688321</v>
+      </c>
+      <c r="G7" s="16">
+        <v>160</v>
+      </c>
+      <c r="H7" s="16">
+        <v>18</v>
+      </c>
+      <c r="I7" s="16">
+        <v>6471.1831476688394</v>
+      </c>
+      <c r="J7" s="16">
+        <v>74.701642036437988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0.76379515680825727</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.89277855417098428</v>
+      </c>
+      <c r="D8" s="16">
+        <v>0.43786982248520712</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.78723404255319152</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0.74267613697109314</v>
+      </c>
+      <c r="G8" s="16">
+        <v>95</v>
+      </c>
+      <c r="H8" s="16">
+        <v>20</v>
+      </c>
+      <c r="I8" s="16">
+        <v>4459.9327099323273</v>
+      </c>
+      <c r="J8" s="16">
+        <v>7.8017473220825195E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="16">
+        <v>0.75689981096408332</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.90765040672696617</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.26101694915254242</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.81914893617021278</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.80113338016704927</v>
+      </c>
+      <c r="G9" s="16">
+        <v>218</v>
+      </c>
+      <c r="H9" s="16">
+        <v>17</v>
+      </c>
+      <c r="I9" s="16">
+        <v>621.48497343063354</v>
+      </c>
+      <c r="J9" s="16">
+        <v>2785.7766802310939</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>0.75051546391752577</v>
+      </c>
+      <c r="C10">
+        <v>0.87229629568425104</v>
+      </c>
+      <c r="D10">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="E10">
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="F10">
+        <v>0.78794303482881833</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>24</v>
+      </c>
+      <c r="I10">
+        <v>238.5943453192711</v>
+      </c>
+      <c r="J10">
+        <v>1.090114831924438</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>0.74743326488706363</v>
+      </c>
+      <c r="C11">
+        <v>0.8722080359889236</v>
+      </c>
+      <c r="D11">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="E11">
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="F11">
+        <v>0.68698419987573189</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>24</v>
+      </c>
+      <c r="I11">
+        <v>39.437344989776612</v>
+      </c>
+      <c r="J11">
+        <v>0.33799505233764648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0.7290679304897314</v>
+      </c>
+      <c r="C12">
+        <v>0.87667989184994954</v>
+      </c>
+      <c r="D12">
+        <v>0.39010989010989011</v>
+      </c>
+      <c r="E12">
+        <v>0.75531914893617025</v>
+      </c>
+      <c r="F12">
+        <v>0.71239305785698559</v>
+      </c>
+      <c r="G12">
+        <v>111</v>
+      </c>
+      <c r="H12">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>3029.172640562057</v>
+      </c>
+      <c r="J12">
+        <v>1.028234481811523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>0.71232876712328763</v>
+      </c>
+      <c r="C13">
+        <v>0.87114891964499319</v>
+      </c>
+      <c r="D13">
+        <v>0.34146341463414642</v>
+      </c>
+      <c r="E13">
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="F13">
+        <v>0.56444419910745947</v>
+      </c>
+      <c r="G13">
+        <v>135</v>
+      </c>
+      <c r="H13">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <v>36006.675769805908</v>
+      </c>
+      <c r="J13">
+        <v>6.1014413833618157E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D60">
+      <c r="B14" s="16">
         <v>0.63778273335457158</v>
       </c>
-      <c r="E60">
+      <c r="C14" s="16">
         <v>0.90329037777778609</v>
       </c>
-      <c r="F60">
+      <c r="D14" s="16">
         <v>9.7591888466413187E-2</v>
       </c>
-      <c r="G60">
+      <c r="E14" s="16">
         <v>0.81914893617021278</v>
       </c>
-      <c r="H60">
+      <c r="F14" s="16">
         <v>0.70210898520029352</v>
       </c>
-      <c r="I60">
+      <c r="G14" s="16">
         <v>712</v>
       </c>
-      <c r="J60">
+      <c r="H14" s="16">
         <v>17</v>
       </c>
-      <c r="K60">
+      <c r="I14" s="16">
         <v>17.717572500705721</v>
       </c>
-      <c r="L60">
+      <c r="J14" s="16">
         <v>0.85363626480102539</v>
       </c>
     </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C61" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D61">
+      <c r="B15">
         <v>0.53429231954790646</v>
       </c>
-      <c r="E61">
+      <c r="C15">
         <v>0.91261952146719916</v>
       </c>
-      <c r="F61">
+      <c r="D15">
         <v>5.1847051198963059E-2</v>
       </c>
-      <c r="G61">
+      <c r="E15">
         <v>0.85106382978723405</v>
       </c>
-      <c r="H61">
+      <c r="F15">
         <v>0.69808028329850547</v>
       </c>
-      <c r="I61">
+      <c r="G15">
         <v>1463</v>
       </c>
-      <c r="J61">
+      <c r="H15">
         <v>14</v>
       </c>
-      <c r="K61">
+      <c r="I15">
         <v>2829.5603652000432</v>
       </c>
-      <c r="L61">
+      <c r="J15">
         <v>0.1520347595214844</v>
       </c>
-      <c r="M61">
-        <v>0.14903450012207031</v>
-      </c>
-    </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C62" s="8"/>
-    </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C63" s="8"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C48:M61">
-    <sortCondition descending="1" ref="D48:D61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J15">
+    <sortCondition descending="1" ref="B2:B15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
VOTING 3 BEST FBETA corrected
</commit_message>
<xml_diff>
--- a/balanced_dataset_results_UPDATED.xlsx
+++ b/balanced_dataset_results_UPDATED.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#coding ground\Github\Repos\fraud_detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aaebd9bc42ac1478/Dokumenty/Edukacja/Data Science/6_DS_Project/Project/03_Coding/fraud_detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11D767D-D93D-48C8-9E06-8FF71280883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E11D767D-D93D-48C8-9E06-8FF71280883B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C6970E-84A0-40CA-9CFA-80B619F70C74}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1350" windowWidth="28800" windowHeight="11775" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -337,13 +337,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -652,9 +645,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -715,7 +708,7 @@
         <v>0.383087158203125</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -747,7 +740,7 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -779,7 +772,7 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -811,7 +804,7 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -843,7 +836,7 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -875,7 +868,7 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -907,7 +900,7 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -939,7 +932,7 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -971,7 +964,7 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1016,9 +1009,9 @@
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1075,7 @@
         <v>0.383087158203125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -1115,7 +1108,7 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1148,7 +1141,7 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -1181,7 +1174,7 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1214,7 +1207,7 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1247,7 +1240,7 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1280,7 +1273,7 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1313,7 +1306,7 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -1346,7 +1339,7 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -1379,7 +1372,7 @@
         <v>3.2007455825805657E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>20</v>
       </c>
@@ -1414,7 +1407,7 @@
         <v>0.40109086036682129</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
@@ -1447,7 +1440,7 @@
         <v>0.34207820892333979</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -1480,7 +1473,7 @@
         <v>1.10018253326416E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
@@ -1513,7 +1506,7 @@
         <v>0.35908150672912598</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -1546,7 +1539,7 @@
         <v>0.28206443786621088</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="1" t="s">
         <v>26</v>
@@ -1579,7 +1572,7 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -1612,7 +1605,7 @@
         <v>0.39809083938598627</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
@@ -1645,7 +1638,7 @@
         <v>0.33907699584960938</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
@@ -1678,7 +1671,7 @@
         <v>1.100277900695801E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="1" t="s">
         <v>30</v>
@@ -1711,7 +1704,7 @@
         <v>0.36808395385742188</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
@@ -1744,7 +1737,7 @@
         <v>0.28406572341918951</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
@@ -1777,7 +1770,7 @@
         <v>1.1002302169799799E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>33</v>
       </c>
@@ -1812,7 +1805,7 @@
         <v>0.46810579299926758</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="1" t="s">
         <v>10</v>
@@ -1845,7 +1838,7 @@
         <v>0.47099637985229492</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="1" t="s">
         <v>11</v>
@@ -1878,7 +1871,7 @@
         <v>1.3003110885620121E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="1" t="s">
         <v>12</v>
@@ -1911,7 +1904,7 @@
         <v>15.430972099304199</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="1" t="s">
         <v>13</v>
@@ -1944,7 +1937,7 @@
         <v>5.5012226104736328E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="1" t="s">
         <v>14</v>
@@ -1977,7 +1970,7 @@
         <v>0.5391232967376709</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="1" t="s">
         <v>15</v>
@@ -2010,7 +2003,7 @@
         <v>8.6019277572631836E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="1" t="s">
         <v>16</v>
@@ -2043,7 +2036,7 @@
         <v>4.7031164169311523E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
@@ -2076,7 +2069,7 @@
         <v>3.4007549285888672E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="1" t="s">
         <v>18</v>
@@ -2109,7 +2102,7 @@
         <v>3.3007383346557617E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>34</v>
       </c>
@@ -2144,7 +2137,7 @@
         <v>0.3140714168548584</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="1" t="s">
         <v>10</v>
@@ -2177,7 +2170,7 @@
         <v>0.32007265090942377</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="1" t="s">
         <v>11</v>
@@ -2210,7 +2203,7 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="1" t="s">
         <v>12</v>
@@ -2243,7 +2236,7 @@
         <v>14.614700794219971</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="1" t="s">
         <v>13</v>
@@ -2276,7 +2269,7 @@
         <v>5.5012702941894531E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="1" t="s">
         <v>14</v>
@@ -2309,7 +2302,7 @@
         <v>0.50911545753479004</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="1" t="s">
         <v>15</v>
@@ -2342,7 +2335,7 @@
         <v>7.3016881942749023E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="B41" s="1" t="s">
         <v>16</v>
@@ -2375,7 +2368,7 @@
         <v>3.8009405136108398E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="1" t="s">
         <v>17</v>
@@ -2408,7 +2401,7 @@
         <v>3.2007217407226563E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="1" t="s">
         <v>18</v>
@@ -2460,14 +2453,14 @@
       <selection activeCell="A16" sqref="A16:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2487,7 +2480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2503,7 @@
         <v>0.53429231954790646</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2533,7 +2526,7 @@
         <v>0.91261952146719916</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2556,7 +2549,7 @@
         <v>5.1847051198963059E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -2579,7 +2572,7 @@
         <v>0.85106382978723405</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -2602,7 +2595,7 @@
         <v>0.69808028329850547</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2625,7 +2618,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -2648,7 +2641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2671,7 +2664,7 @@
         <v>2829.5603652000432</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -2694,7 +2687,7 @@
         <v>0.1520347595214844</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2717,7 +2710,7 @@
         <v>0.14903450012207031</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2742,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -2784,7 +2777,7 @@
         <v>1.10015869140625E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2819,7 +2812,7 @@
         <v>74.969163417816162</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -2854,7 +2847,7 @@
         <v>6.3014507293701172E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2889,7 +2882,7 @@
         <v>1.032234668731689</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -2924,7 +2917,7 @@
         <v>5.9012651443481452E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -2972,22 +2965,22 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3016,7 +3009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>AVERAGE(D3:D12)</f>
         <v>0.76506404331409994</v>
@@ -3058,7 +3051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
@@ -3096,7 +3089,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
@@ -3134,7 +3127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
@@ -3172,7 +3165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>33</v>
       </c>
@@ -3210,7 +3203,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
@@ -3248,7 +3241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
@@ -3286,7 +3279,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
@@ -3324,7 +3317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -3359,7 +3352,7 @@
         <v>0.39809083938598627</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3394,7 +3387,7 @@
         <v>4.0008783340454102E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>AVERAGE(D13:D22)</f>
         <v>0.73055183944449764</v>
@@ -3433,7 +3426,7 @@
         <v>3.4007549285888672E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
@@ -3468,7 +3461,7 @@
         <v>4.7031164169311523E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
@@ -3503,7 +3496,7 @@
         <v>1.3003110885620121E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
@@ -3538,7 +3531,7 @@
         <v>0.3140714168548584</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3573,7 +3566,7 @@
         <v>0.40109086036682129</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -3608,7 +3601,7 @@
         <v>3.5007953643798828E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3636,7 @@
         <v>0.36808395385742188</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3678,7 +3671,7 @@
         <v>0.35908150672912598</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
@@ -3713,7 +3706,7 @@
         <v>0.383087158203125</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -3748,7 +3741,7 @@
         <v>3.1007289886474609E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>AVERAGE(D23:D34)</f>
         <v>0.64199376937573627</v>
@@ -3787,7 +3780,7 @@
         <v>0.32007265090942377</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
@@ -3822,7 +3815,7 @@
         <v>7.7994539737701416</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
@@ -3857,7 +3850,7 @@
         <v>3.2007455825805657E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
@@ -3892,7 +3885,7 @@
         <v>0.50911545753479004</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
@@ -3927,7 +3920,7 @@
         <v>0.5391232967376709</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>19</v>
       </c>
@@ -3962,7 +3955,7 @@
         <v>0.53112077713012695</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
@@ -3997,7 +3990,7 @@
         <v>3.3007383346557617E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -4032,7 +4025,7 @@
         <v>0.28406572341918951</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -4067,7 +4060,7 @@
         <v>0.28206443786621088</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>19</v>
       </c>
@@ -4102,7 +4095,7 @@
         <v>1.2002706527709959E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
@@ -4137,7 +4130,7 @@
         <v>0.29306674003601069</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
@@ -4172,7 +4165,7 @@
         <v>1.100254058837891E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>AVERAGE(D35:D44)</f>
         <v>0.35857142738267272</v>
@@ -4211,7 +4204,7 @@
         <v>0.33907699584960938</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>20</v>
       </c>
@@ -4246,7 +4239,7 @@
         <v>0.34207820892333979</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
@@ -4281,7 +4274,7 @@
         <v>8.6019277572631836E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
@@ -4316,7 +4309,7 @@
         <v>7.7017784118652344E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
@@ -4351,7 +4344,7 @@
         <v>7.3016881942749023E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>19</v>
       </c>
@@ -4386,7 +4379,7 @@
         <v>5.4012060165405273E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>20</v>
       </c>
@@ -4421,7 +4414,7 @@
         <v>1.10018253326416E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>34</v>
       </c>
@@ -4456,7 +4449,7 @@
         <v>5.5012702941894531E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>20</v>
       </c>
@@ -4491,7 +4484,7 @@
         <v>1.100277900695801E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>33</v>
       </c>
@@ -4526,7 +4519,7 @@
         <v>5.5012226104736328E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D47" s="1" t="s">
         <v>0</v>
       </c>
@@ -4558,7 +4551,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B48" s="8"/>
       <c r="C48" s="1" t="s">
         <v>40</v>
@@ -4594,7 +4587,7 @@
         <v>0.14903450012207031</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
       <c r="C49" s="4" t="s">
         <v>49</v>
@@ -4627,7 +4620,7 @@
         <v>2785.7766802310939</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
       <c r="C50" s="3" t="s">
         <v>50</v>
@@ -4660,7 +4653,7 @@
         <v>0.85363626480102539</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="10"/>
       <c r="C51" s="4" t="s">
         <v>53</v>
@@ -4693,7 +4686,7 @@
         <v>6.2342522144317627</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="8"/>
       <c r="C52" s="6" t="s">
         <v>36</v>
@@ -4729,7 +4722,7 @@
         <v>74.969163417816162</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="8"/>
       <c r="C53" s="6" t="s">
         <v>35</v>
@@ -4765,7 +4758,7 @@
         <v>1.10015869140625E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
       <c r="C54" s="3" t="s">
         <v>51</v>
@@ -4798,7 +4791,7 @@
         <v>1.173768281936646</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="8"/>
       <c r="C55" s="1" t="s">
         <v>37</v>
@@ -4834,7 +4827,7 @@
         <v>6.3014507293701172E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
       <c r="C56" s="3" t="s">
         <v>48</v>
@@ -4867,7 +4860,7 @@
         <v>10.52744150161743</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="10"/>
       <c r="C57" s="3" t="s">
         <v>52</v>
@@ -4900,7 +4893,7 @@
         <v>1.2859871387481689</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="8"/>
       <c r="C58" s="1" t="s">
         <v>38</v>
@@ -4936,7 +4929,7 @@
         <v>1.032234668731689</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="10"/>
       <c r="C59" s="3" t="s">
         <v>55</v>
@@ -4969,7 +4962,7 @@
         <v>1.090114831924438</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B60" s="10"/>
       <c r="C60" s="3" t="s">
         <v>54</v>
@@ -5002,7 +4995,7 @@
         <v>0.33799505233764648</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B61" s="8"/>
       <c r="C61" s="1" t="s">
         <v>39</v>
@@ -5038,10 +5031,10 @@
         <v>5.9012651443481452E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C62" s="7"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C63" s="7"/>
     </row>
   </sheetData>
@@ -5057,22 +5050,22 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A4" sqref="A4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5101,103 +5094,103 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2">
         <v>0.79741727199354318</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2">
         <v>0.90379636873323299</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2">
         <v>0.59375</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2">
         <v>0.80851063829787229</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2">
         <v>0.77776653446199817</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2">
         <v>52</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2">
         <v>18</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2">
         <v>204.73599044481909</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2">
         <v>6.2342522144317627</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3">
         <v>0.79046836483155314</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3">
         <v>0.89352876158126815</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3">
         <v>0.88095238095238093</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3">
         <v>0.78723404255319152</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3">
         <v>0.80511414406811932</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3">
         <v>20</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3">
         <v>628.83125205039983</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3">
         <v>1.173768281936646</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="16">
-        <v>0.77978635990139689</v>
-      </c>
-      <c r="C4" s="16">
-        <v>0.88820078667556523</v>
-      </c>
-      <c r="D4" s="16">
-        <v>0.86904761904761907</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="B4">
+        <v>0.78010686395396633</v>
+      </c>
+      <c r="C4">
+        <v>0.88820961264509801</v>
+      </c>
+      <c r="D4">
+        <v>0.87951807228915657</v>
+      </c>
+      <c r="E4">
         <v>0.77659574468085102</v>
       </c>
-      <c r="F4" s="16">
-        <v>0.80735210915347733</v>
-      </c>
-      <c r="G4" s="16">
-        <v>11</v>
-      </c>
-      <c r="H4" s="16">
+      <c r="F4">
+        <v>0.80683498090524919</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
         <v>21</v>
       </c>
-      <c r="I4" s="16">
-        <v>1341.127286195755</v>
-      </c>
-      <c r="J4" s="16">
-        <v>10.52744150161743</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1083.818585634232</v>
+      </c>
+      <c r="J4">
+        <v>8.5441548824310303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
@@ -5229,135 +5222,135 @@
         <v>1.2859871387481689</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6">
         <v>0.77442414614773636</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6">
         <v>0.89811535504621998</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6">
         <v>0.44642857142857151</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6">
         <v>0.7978723404255319</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6">
         <v>0.6929470987941333</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6">
         <v>93</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6">
         <v>19</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6">
         <v>797.83375072479248</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6">
         <v>1.300382614135742E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7">
         <v>0.76411446249033255</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7">
         <v>0.90284316402369558</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7">
         <v>0.32203389830508472</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7">
         <v>0.80851063829787229</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7">
         <v>0.63109300844688321</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7">
         <v>160</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7">
         <v>18</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7">
         <v>6471.1831476688394</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7">
         <v>74.701642036437988</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8">
         <v>0.76379515680825727</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8">
         <v>0.89277855417098428</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8">
         <v>0.43786982248520712</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8">
         <v>0.78723404255319152</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8">
         <v>0.74267613697109314</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8">
         <v>95</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8">
         <v>20</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8">
         <v>4459.9327099323273</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8">
         <v>7.8017473220825195E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9">
         <v>0.75689981096408332</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9">
         <v>0.90765040672696617</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9">
         <v>0.26101694915254242</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9">
         <v>0.81914893617021278</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9">
         <v>0.80113338016704927</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9">
         <v>218</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9">
         <v>17</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9">
         <v>621.48497343063354</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9">
         <v>2785.7766802310939</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>55</v>
       </c>
@@ -5389,7 +5382,7 @@
         <v>1.090114831924438</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
@@ -5421,7 +5414,7 @@
         <v>0.33799505233764648</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -5453,7 +5446,7 @@
         <v>1.028234481811523</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -5485,39 +5478,39 @@
         <v>6.1014413833618157E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14">
         <v>0.63778273335457158</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14">
         <v>0.90329037777778609</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14">
         <v>9.7591888466413187E-2</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14">
         <v>0.81914893617021278</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14">
         <v>0.70210898520029352</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14">
         <v>712</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14">
         <v>17</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14">
         <v>17.717572500705721</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14">
         <v>0.85363626480102539</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>

</xml_diff>